<commit_message>
correccion en reporte mensual
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/flujoefectivomensual3B.xlsx
+++ b/public/application/files/jasper/templates/flujoefectivomensual3B.xlsx
@@ -278,7 +278,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -290,17 +290,14 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -310,22 +307,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -663,7 +664,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -672,66 +673,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.75" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="29.75" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="28">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" ht="22.25" customHeight="1">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="18">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1">
       <c r="A7" s="1" t="s">
@@ -757,72 +758,72 @@
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="20" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="19" t="s">
         <v>27</v>
       </c>
     </row>
@@ -838,7 +839,6 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>